<commit_message>
Fixed various Mu editor code formatting issues and checks
</commit_message>
<xml_diff>
--- a/Documentation/Parts.xlsx
+++ b/Documentation/Parts.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Armachat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Armachat\Armachat-circuitpython\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECACE12-3B10-45F6-B142-8EEEA817CB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967EF99C-F5BD-4A96-965F-6D5C4CF4063C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{804B02E0-43F0-4DAF-86C6-ACAAAC73CD2E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{804B02E0-43F0-4DAF-86C6-ACAAAC73CD2E}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="2" r:id="rId1"/>
     <sheet name="Pico GPIO" sheetId="3" r:id="rId2"/>
     <sheet name="Keypad" sheetId="4" r:id="rId3"/>
-    <sheet name="Screens and Keys" sheetId="5" r:id="rId4"/>
+    <sheet name="Keypad (Col, Row)" sheetId="6" r:id="rId4"/>
+    <sheet name="Screens and Keys" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">BOM!$A$1:$J$27</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="227">
   <si>
     <t>Description</t>
   </si>
@@ -697,6 +698,30 @@
   </si>
   <si>
     <t>LoRa Antenna (SMA)</t>
+  </si>
+  <si>
+    <t>Key &amp; Array Indexes</t>
+  </si>
+  <si>
+    <t>Rows</t>
+  </si>
+  <si>
+    <t>Columns</t>
+  </si>
+  <si>
+    <t>Keys</t>
+  </si>
+  <si>
+    <t>Key &amp; IO</t>
+  </si>
+  <si>
+    <t>Boot</t>
+  </si>
+  <si>
+    <t>Safe Mode</t>
+  </si>
+  <si>
+    <t>Write Mode</t>
   </si>
 </sst>
 </file>
@@ -738,7 +763,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -754,6 +779,42 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -804,7 +865,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -846,6 +907,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1169,7 +1260,7 @@
   </sheetPr>
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1991,8 +2082,8 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2628,7 +2719,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3076,11 +3167,976 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638AD3B4-41B9-45BA-A561-4767E27251F2}">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79560918-82E4-46AF-B408-379D6C110666}">
+  <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="L1" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="R2" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="S2" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="U2" s="21" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="O3" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="P3" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q3" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="R3" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="S3" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="L4" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="M4" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="N4" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="O4" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="P4" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q4" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="R4" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="S4" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="T4" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="U4" s="21" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="L6" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="23"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="24">
+        <v>0</v>
+      </c>
+      <c r="B7" s="26">
+        <v>1</v>
+      </c>
+      <c r="C7" s="28">
+        <v>2</v>
+      </c>
+      <c r="D7" s="25">
+        <v>3</v>
+      </c>
+      <c r="E7" s="27">
+        <v>4</v>
+      </c>
+      <c r="F7" s="27">
+        <v>4</v>
+      </c>
+      <c r="G7" s="25">
+        <v>3</v>
+      </c>
+      <c r="H7" s="28">
+        <v>2</v>
+      </c>
+      <c r="I7" s="26">
+        <v>1</v>
+      </c>
+      <c r="J7" s="24">
+        <v>0</v>
+      </c>
+      <c r="L7" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="M7" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="N7" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="O7" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="P7" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q7" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="R7" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="S7" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="T7" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="U7" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="24">
+        <v>0</v>
+      </c>
+      <c r="B8" s="26">
+        <v>1</v>
+      </c>
+      <c r="C8" s="28">
+        <v>2</v>
+      </c>
+      <c r="D8" s="25">
+        <v>3</v>
+      </c>
+      <c r="E8" s="27">
+        <v>4</v>
+      </c>
+      <c r="F8" s="27">
+        <v>4</v>
+      </c>
+      <c r="G8" s="25">
+        <v>3</v>
+      </c>
+      <c r="H8" s="28">
+        <v>2</v>
+      </c>
+      <c r="I8" s="26">
+        <v>1</v>
+      </c>
+      <c r="J8" s="24">
+        <v>0</v>
+      </c>
+      <c r="L8" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="M8" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="N8" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="O8" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="P8" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q8" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="R8" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="S8" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="T8" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="U8" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>0</v>
+      </c>
+      <c r="B9" s="26">
+        <v>1</v>
+      </c>
+      <c r="C9" s="28">
+        <v>2</v>
+      </c>
+      <c r="D9" s="25">
+        <v>3</v>
+      </c>
+      <c r="E9" s="27">
+        <v>4</v>
+      </c>
+      <c r="F9" s="27">
+        <v>4</v>
+      </c>
+      <c r="G9" s="25">
+        <v>3</v>
+      </c>
+      <c r="H9" s="28">
+        <v>2</v>
+      </c>
+      <c r="I9" s="26">
+        <v>1</v>
+      </c>
+      <c r="J9" s="24">
+        <v>0</v>
+      </c>
+      <c r="L9" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="M9" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="N9" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="O9" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="P9" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q9" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="R9" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="S9" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="T9" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="U9" s="30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="17"/>
+      <c r="U10" s="17"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="L11" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="23"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="29">
+        <v>5</v>
+      </c>
+      <c r="B12" s="29">
+        <v>5</v>
+      </c>
+      <c r="C12" s="29">
+        <v>5</v>
+      </c>
+      <c r="D12" s="29">
+        <v>5</v>
+      </c>
+      <c r="E12" s="29">
+        <v>5</v>
+      </c>
+      <c r="F12" s="28">
+        <v>2</v>
+      </c>
+      <c r="G12" s="28">
+        <v>2</v>
+      </c>
+      <c r="H12" s="28">
+        <v>2</v>
+      </c>
+      <c r="I12" s="28">
+        <v>2</v>
+      </c>
+      <c r="J12" s="28">
+        <v>2</v>
+      </c>
+      <c r="L12" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="M12" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="N12" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="O12" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="P12" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q12" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="R12" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="S12" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="T12" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="U12" s="32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="27">
+        <v>4</v>
+      </c>
+      <c r="B13" s="27">
+        <v>4</v>
+      </c>
+      <c r="C13" s="27">
+        <v>4</v>
+      </c>
+      <c r="D13" s="27">
+        <v>4</v>
+      </c>
+      <c r="E13" s="27">
+        <v>4</v>
+      </c>
+      <c r="F13" s="26">
+        <v>1</v>
+      </c>
+      <c r="G13" s="26">
+        <v>1</v>
+      </c>
+      <c r="H13" s="26">
+        <v>1</v>
+      </c>
+      <c r="I13" s="26">
+        <v>1</v>
+      </c>
+      <c r="J13" s="26">
+        <v>1</v>
+      </c>
+      <c r="L13" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="M13" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="N13" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="O13" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="P13" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q13" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="R13" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="S13" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="T13" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="U13" s="31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="25">
+        <v>3</v>
+      </c>
+      <c r="B14" s="25">
+        <v>3</v>
+      </c>
+      <c r="C14" s="25">
+        <v>3</v>
+      </c>
+      <c r="D14" s="25">
+        <v>3</v>
+      </c>
+      <c r="E14" s="25">
+        <v>3</v>
+      </c>
+      <c r="F14" s="24">
+        <v>0</v>
+      </c>
+      <c r="G14" s="24">
+        <v>0</v>
+      </c>
+      <c r="H14" s="24">
+        <v>0</v>
+      </c>
+      <c r="I14" s="24">
+        <v>0</v>
+      </c>
+      <c r="J14" s="24">
+        <v>0</v>
+      </c>
+      <c r="L14" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="M14" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="N14" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="O14" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="P14" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q14" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="R14" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="S14" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="T14" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="U14" s="30" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="L16" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="23"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="str">
+        <f>A2 &amp; " (" &amp; A7 &amp; ", " &amp; A12 &amp; ")"</f>
+        <v>Q (0, 5)</v>
+      </c>
+      <c r="B17" s="21" t="str">
+        <f>B2 &amp; " (" &amp; B7 &amp; ", " &amp; B12 &amp; ")"</f>
+        <v>W (1, 5)</v>
+      </c>
+      <c r="C17" s="21" t="str">
+        <f>C2 &amp; " (" &amp; C7 &amp; ", " &amp; C12 &amp; ")"</f>
+        <v>E (2, 5)</v>
+      </c>
+      <c r="D17" s="21" t="str">
+        <f>D2 &amp; " (" &amp; D7 &amp; ", " &amp; D12 &amp; ")"</f>
+        <v>R (3, 5)</v>
+      </c>
+      <c r="E17" s="21" t="str">
+        <f>E2 &amp; " (" &amp; E7 &amp; ", " &amp; E12 &amp; ")"</f>
+        <v>T (4, 5)</v>
+      </c>
+      <c r="F17" s="21" t="str">
+        <f>F2 &amp; " (" &amp; F7 &amp; ", " &amp; F12 &amp; ")"</f>
+        <v>Y (4, 2)</v>
+      </c>
+      <c r="G17" s="21" t="str">
+        <f>G2 &amp; " (" &amp; G7 &amp; ", " &amp; G12 &amp; ")"</f>
+        <v>U (3, 2)</v>
+      </c>
+      <c r="H17" s="21" t="str">
+        <f>H2 &amp; " (" &amp; H7 &amp; ", " &amp; H12 &amp; ")"</f>
+        <v>I (2, 2)</v>
+      </c>
+      <c r="I17" s="21" t="str">
+        <f>I2 &amp; " (" &amp; I7 &amp; ", " &amp; I12 &amp; ")"</f>
+        <v>O (1, 2)</v>
+      </c>
+      <c r="J17" s="21" t="str">
+        <f>J2 &amp; " (" &amp; J7 &amp; ", " &amp; J12 &amp; ")"</f>
+        <v>P (0, 2)</v>
+      </c>
+      <c r="L17" s="21" t="str">
+        <f>L2 &amp; " (" &amp; L7 &amp; ", " &amp; L12 &amp; ")"</f>
+        <v>Q (GP1, GP22)</v>
+      </c>
+      <c r="M17" s="21" t="str">
+        <f>M2 &amp; " (" &amp; M7 &amp; ", " &amp; M12 &amp; ")"</f>
+        <v>W (GP2, GP22)</v>
+      </c>
+      <c r="N17" s="21" t="str">
+        <f>N2 &amp; " (" &amp; N7 &amp; ", " &amp; N12 &amp; ")"</f>
+        <v>E (GP3, GP22)</v>
+      </c>
+      <c r="O17" s="21" t="str">
+        <f>O2 &amp; " (" &amp; O7 &amp; ", " &amp; O12 &amp; ")"</f>
+        <v>R (GP4, GP22)</v>
+      </c>
+      <c r="P17" s="21" t="str">
+        <f>P2 &amp; " (" &amp; P7 &amp; ", " &amp; P12 &amp; ")"</f>
+        <v>T (GP5, GP22)</v>
+      </c>
+      <c r="Q17" s="21" t="str">
+        <f>Q2 &amp; " (" &amp; Q7 &amp; ", " &amp; Q12 &amp; ")"</f>
+        <v>Y (GP5, GP15)</v>
+      </c>
+      <c r="R17" s="21" t="str">
+        <f>R2 &amp; " (" &amp; R7 &amp; ", " &amp; R12 &amp; ")"</f>
+        <v>U (GP4, GP15)</v>
+      </c>
+      <c r="S17" s="21" t="str">
+        <f>S2 &amp; " (" &amp; S7 &amp; ", " &amp; S12 &amp; ")"</f>
+        <v>I (GP3, GP15)</v>
+      </c>
+      <c r="T17" s="21" t="str">
+        <f>T2 &amp; " (" &amp; T7 &amp; ", " &amp; T12 &amp; ")"</f>
+        <v>O (GP2, GP15)</v>
+      </c>
+      <c r="U17" s="21" t="str">
+        <f>U2 &amp; " (" &amp; U7 &amp; ", " &amp; U12 &amp; ")"</f>
+        <v>P (GP1, GP15)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="str">
+        <f>A3 &amp; " (" &amp; A8 &amp; ", " &amp; A13 &amp; ")"</f>
+        <v>A (0, 4)</v>
+      </c>
+      <c r="B18" s="21" t="str">
+        <f>B3 &amp; " (" &amp; B8 &amp; ", " &amp; B13 &amp; ")"</f>
+        <v>S (1, 4)</v>
+      </c>
+      <c r="C18" s="21" t="str">
+        <f>C3 &amp; " (" &amp; C8 &amp; ", " &amp; C13 &amp; ")"</f>
+        <v>D (2, 4)</v>
+      </c>
+      <c r="D18" s="21" t="str">
+        <f>D3 &amp; " (" &amp; D8 &amp; ", " &amp; D13 &amp; ")"</f>
+        <v>F (3, 4)</v>
+      </c>
+      <c r="E18" s="21" t="str">
+        <f>E3 &amp; " (" &amp; E8 &amp; ", " &amp; E13 &amp; ")"</f>
+        <v>G (4, 4)</v>
+      </c>
+      <c r="F18" s="21" t="str">
+        <f>F3 &amp; " (" &amp; F8 &amp; ", " &amp; F13 &amp; ")"</f>
+        <v>H (4, 1)</v>
+      </c>
+      <c r="G18" s="21" t="str">
+        <f>G3 &amp; " (" &amp; G8 &amp; ", " &amp; G13 &amp; ")"</f>
+        <v>J (3, 1)</v>
+      </c>
+      <c r="H18" s="21" t="str">
+        <f>H3 &amp; " (" &amp; H8 &amp; ", " &amp; H13 &amp; ")"</f>
+        <v>K (2, 1)</v>
+      </c>
+      <c r="I18" s="21" t="str">
+        <f>I3 &amp; " (" &amp; I8 &amp; ", " &amp; I13 &amp; ")"</f>
+        <v>L (1, 1)</v>
+      </c>
+      <c r="J18" s="21" t="str">
+        <f>J3 &amp; " (" &amp; J8 &amp; ", " &amp; J13 &amp; ")"</f>
+        <v>DEL (0, 1)</v>
+      </c>
+      <c r="L18" s="21" t="str">
+        <f>L3 &amp; " (" &amp; L8 &amp; ", " &amp; L13 &amp; ")"</f>
+        <v>A (GP1, GP7)</v>
+      </c>
+      <c r="M18" s="21" t="str">
+        <f>M3 &amp; " (" &amp; M8 &amp; ", " &amp; M13 &amp; ")"</f>
+        <v>S (GP2, GP7)</v>
+      </c>
+      <c r="N18" s="21" t="str">
+        <f>N3 &amp; " (" &amp; N8 &amp; ", " &amp; N13 &amp; ")"</f>
+        <v>D (GP3, GP7)</v>
+      </c>
+      <c r="O18" s="21" t="str">
+        <f>O3 &amp; " (" &amp; O8 &amp; ", " &amp; O13 &amp; ")"</f>
+        <v>F (GP4, GP7)</v>
+      </c>
+      <c r="P18" s="21" t="str">
+        <f>P3 &amp; " (" &amp; P8 &amp; ", " &amp; P13 &amp; ")"</f>
+        <v>G (GP5, GP7)</v>
+      </c>
+      <c r="Q18" s="21" t="str">
+        <f>Q3 &amp; " (" &amp; Q8 &amp; ", " &amp; Q13 &amp; ")"</f>
+        <v>H (GP5, GP9)</v>
+      </c>
+      <c r="R18" s="21" t="str">
+        <f>R3 &amp; " (" &amp; R8 &amp; ", " &amp; R13 &amp; ")"</f>
+        <v>J (GP4, GP9)</v>
+      </c>
+      <c r="S18" s="21" t="str">
+        <f>S3 &amp; " (" &amp; S8 &amp; ", " &amp; S13 &amp; ")"</f>
+        <v>K (GP3, GP9)</v>
+      </c>
+      <c r="T18" s="21" t="str">
+        <f>T3 &amp; " (" &amp; T8 &amp; ", " &amp; T13 &amp; ")"</f>
+        <v>L (GP2, GP9)</v>
+      </c>
+      <c r="U18" s="21" t="str">
+        <f>U3 &amp; " (" &amp; U8 &amp; ", " &amp; U13 &amp; ")"</f>
+        <v>DEL (GP1, GP9)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="str">
+        <f>A4 &amp; " (" &amp; A9 &amp; ", " &amp; A14 &amp; ")"</f>
+        <v>ALT (0, 3)</v>
+      </c>
+      <c r="B19" s="21" t="str">
+        <f>B4 &amp; " (" &amp; B9 &amp; ", " &amp; B14 &amp; ")"</f>
+        <v>Z (1, 3)</v>
+      </c>
+      <c r="C19" s="21" t="str">
+        <f>C4 &amp; " (" &amp; C9 &amp; ", " &amp; C14 &amp; ")"</f>
+        <v>X (2, 3)</v>
+      </c>
+      <c r="D19" s="21" t="str">
+        <f>D4 &amp; " (" &amp; D9 &amp; ", " &amp; D14 &amp; ")"</f>
+        <v>C (3, 3)</v>
+      </c>
+      <c r="E19" s="21" t="str">
+        <f>E4 &amp; " (" &amp; E9 &amp; ", " &amp; E14 &amp; ")"</f>
+        <v>V (4, 3)</v>
+      </c>
+      <c r="F19" s="21" t="str">
+        <f>F4 &amp; " (" &amp; F9 &amp; ", " &amp; F14 &amp; ")"</f>
+        <v>B (4, 0)</v>
+      </c>
+      <c r="G19" s="21" t="str">
+        <f>G4 &amp; " (" &amp; G9 &amp; ", " &amp; G14 &amp; ")"</f>
+        <v>N (3, 0)</v>
+      </c>
+      <c r="H19" s="21" t="str">
+        <f>H4 &amp; " (" &amp; H9 &amp; ", " &amp; H14 &amp; ")"</f>
+        <v>M (2, 0)</v>
+      </c>
+      <c r="I19" s="21" t="str">
+        <f>I4 &amp; " (" &amp; I9 &amp; ", " &amp; I14 &amp; ")"</f>
+        <v>SPC (1, 0)</v>
+      </c>
+      <c r="J19" s="21" t="str">
+        <f>J4 &amp; " (" &amp; J9 &amp; ", " &amp; J14 &amp; ")"</f>
+        <v>ENT (0, 0)</v>
+      </c>
+      <c r="L19" s="21" t="str">
+        <f>L4 &amp; " (" &amp; L9 &amp; ", " &amp; L14 &amp; ")"</f>
+        <v>ALT (GP1, GP8)</v>
+      </c>
+      <c r="M19" s="21" t="str">
+        <f>M4 &amp; " (" &amp; M9 &amp; ", " &amp; M14 &amp; ")"</f>
+        <v>Z (GP2, GP8)</v>
+      </c>
+      <c r="N19" s="21" t="str">
+        <f>N4 &amp; " (" &amp; N9 &amp; ", " &amp; N14 &amp; ")"</f>
+        <v>X (GP3, GP8)</v>
+      </c>
+      <c r="O19" s="21" t="str">
+        <f>O4 &amp; " (" &amp; O9 &amp; ", " &amp; O14 &amp; ")"</f>
+        <v>C (GP4, GP8)</v>
+      </c>
+      <c r="P19" s="21" t="str">
+        <f>P4 &amp; " (" &amp; P9 &amp; ", " &amp; P14 &amp; ")"</f>
+        <v>V (GP5, GP8)</v>
+      </c>
+      <c r="Q19" s="21" t="str">
+        <f>Q4 &amp; " (" &amp; Q9 &amp; ", " &amp; Q14 &amp; ")"</f>
+        <v>B (GP5, GP6)</v>
+      </c>
+      <c r="R19" s="21" t="str">
+        <f>R4 &amp; " (" &amp; R9 &amp; ", " &amp; R14 &amp; ")"</f>
+        <v>N (GP4, GP6)</v>
+      </c>
+      <c r="S19" s="21" t="str">
+        <f>S4 &amp; " (" &amp; S9 &amp; ", " &amp; S14 &amp; ")"</f>
+        <v>M (GP3, GP6)</v>
+      </c>
+      <c r="T19" s="21" t="str">
+        <f>T4 &amp; " (" &amp; T9 &amp; ", " &amp; T14 &amp; ")"</f>
+        <v>SPC (GP2, GP6)</v>
+      </c>
+      <c r="U19" s="21" t="str">
+        <f>U4 &amp; " (" &amp; U9 &amp; ", " &amp; U14 &amp; ")"</f>
+        <v>ENT (GP1, GP6)</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="L1:U1"/>
+    <mergeCell ref="L6:U6"/>
+    <mergeCell ref="L11:U11"/>
+    <mergeCell ref="L16:U16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638AD3B4-41B9-45BA-A561-4767E27251F2}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3099,26 +4155,26 @@
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="B3" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C3" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3126,10 +4182,10 @@
         <v>206</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="C4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3137,10 +4193,10 @@
         <v>206</v>
       </c>
       <c r="B5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C5" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3148,10 +4204,10 @@
         <v>206</v>
       </c>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3159,10 +4215,10 @@
         <v>206</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="C7" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3170,10 +4226,10 @@
         <v>206</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C8" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3181,10 +4237,10 @@
         <v>206</v>
       </c>
       <c r="B9" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3192,10 +4248,10 @@
         <v>206</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="C10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3203,9 +4259,31 @@
         <v>206</v>
       </c>
       <c r="B11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>206</v>
+      </c>
+      <c r="B12" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>206</v>
+      </c>
+      <c r="B13" t="s">
         <v>161</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C13" t="s">
         <v>216</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed a bugs with displaying messages after sending a message
</commit_message>
<xml_diff>
--- a/Documentation/Parts.xlsx
+++ b/Documentation/Parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Armachat\Armachat-circuitpython\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967EF99C-F5BD-4A96-965F-6D5C4CF4063C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130B10B1-E3DD-444D-8A5A-449F3055A1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{804B02E0-43F0-4DAF-86C6-ACAAAC73CD2E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{804B02E0-43F0-4DAF-86C6-ACAAAC73CD2E}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Keypad" sheetId="4" r:id="rId3"/>
     <sheet name="Keypad (Col, Row)" sheetId="6" r:id="rId4"/>
     <sheet name="Screens and Keys" sheetId="5" r:id="rId5"/>
+    <sheet name="Messages" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">BOM!$A$1:$J$27</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="245">
   <si>
     <t>Description</t>
   </si>
@@ -722,6 +723,60 @@
   </si>
   <si>
     <t>Write Mode</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>a3</t>
+  </si>
+  <si>
+    <t>a4</t>
+  </si>
+  <si>
+    <t>a5</t>
+  </si>
+  <si>
+    <t>a6</t>
+  </si>
+  <si>
+    <t>a7</t>
+  </si>
+  <si>
+    <t>a8</t>
+  </si>
+  <si>
+    <t>b76ab505</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>destination</t>
+  </si>
+  <si>
+    <t>sender</t>
+  </si>
+  <si>
+    <t>messageID</t>
+  </si>
+  <si>
+    <t>hop</t>
+  </si>
+  <si>
+    <t>rssi</t>
+  </si>
+  <si>
+    <t>snr</t>
+  </si>
+  <si>
+    <t>timeStamp</t>
+  </si>
+  <si>
+    <t>packet_text</t>
   </si>
 </sst>
 </file>
@@ -865,7 +920,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -937,6 +992,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3196,30 +3254,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="37" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="L1" s="23" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="L1" s="37" t="s">
         <v>222</v>
       </c>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
@@ -3408,30 +3466,30 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="37" t="s">
         <v>221</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="L6" s="23" t="s">
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="L6" s="37" t="s">
         <v>221</v>
       </c>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="37"/>
+      <c r="U6" s="37"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="24">
@@ -3632,30 +3690,30 @@
       <c r="U10" s="17"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="L11" s="23" t="s">
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="L11" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="37"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="37"/>
+      <c r="R11" s="37"/>
+      <c r="S11" s="37"/>
+      <c r="T11" s="37"/>
+      <c r="U11" s="37"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
@@ -3844,274 +3902,274 @@
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="L16" s="23" t="s">
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="L16" s="37" t="s">
         <v>223</v>
       </c>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="23"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="37"/>
+      <c r="R16" s="37"/>
+      <c r="S16" s="37"/>
+      <c r="T16" s="37"/>
+      <c r="U16" s="37"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="str">
-        <f>A2 &amp; " (" &amp; A7 &amp; ", " &amp; A12 &amp; ")"</f>
+        <f t="shared" ref="A17:J17" si="0">A2 &amp; " (" &amp; A7 &amp; ", " &amp; A12 &amp; ")"</f>
         <v>Q (0, 5)</v>
       </c>
       <c r="B17" s="21" t="str">
-        <f>B2 &amp; " (" &amp; B7 &amp; ", " &amp; B12 &amp; ")"</f>
+        <f t="shared" si="0"/>
         <v>W (1, 5)</v>
       </c>
       <c r="C17" s="21" t="str">
-        <f>C2 &amp; " (" &amp; C7 &amp; ", " &amp; C12 &amp; ")"</f>
+        <f t="shared" si="0"/>
         <v>E (2, 5)</v>
       </c>
       <c r="D17" s="21" t="str">
-        <f>D2 &amp; " (" &amp; D7 &amp; ", " &amp; D12 &amp; ")"</f>
+        <f t="shared" si="0"/>
         <v>R (3, 5)</v>
       </c>
       <c r="E17" s="21" t="str">
-        <f>E2 &amp; " (" &amp; E7 &amp; ", " &amp; E12 &amp; ")"</f>
+        <f t="shared" si="0"/>
         <v>T (4, 5)</v>
       </c>
       <c r="F17" s="21" t="str">
-        <f>F2 &amp; " (" &amp; F7 &amp; ", " &amp; F12 &amp; ")"</f>
+        <f t="shared" si="0"/>
         <v>Y (4, 2)</v>
       </c>
       <c r="G17" s="21" t="str">
-        <f>G2 &amp; " (" &amp; G7 &amp; ", " &amp; G12 &amp; ")"</f>
+        <f t="shared" si="0"/>
         <v>U (3, 2)</v>
       </c>
       <c r="H17" s="21" t="str">
-        <f>H2 &amp; " (" &amp; H7 &amp; ", " &amp; H12 &amp; ")"</f>
+        <f t="shared" si="0"/>
         <v>I (2, 2)</v>
       </c>
       <c r="I17" s="21" t="str">
-        <f>I2 &amp; " (" &amp; I7 &amp; ", " &amp; I12 &amp; ")"</f>
+        <f t="shared" si="0"/>
         <v>O (1, 2)</v>
       </c>
       <c r="J17" s="21" t="str">
-        <f>J2 &amp; " (" &amp; J7 &amp; ", " &amp; J12 &amp; ")"</f>
+        <f t="shared" si="0"/>
         <v>P (0, 2)</v>
       </c>
       <c r="L17" s="21" t="str">
-        <f>L2 &amp; " (" &amp; L7 &amp; ", " &amp; L12 &amp; ")"</f>
+        <f t="shared" ref="L17:U17" si="1">L2 &amp; " (" &amp; L7 &amp; ", " &amp; L12 &amp; ")"</f>
         <v>Q (GP1, GP22)</v>
       </c>
       <c r="M17" s="21" t="str">
-        <f>M2 &amp; " (" &amp; M7 &amp; ", " &amp; M12 &amp; ")"</f>
+        <f t="shared" si="1"/>
         <v>W (GP2, GP22)</v>
       </c>
       <c r="N17" s="21" t="str">
-        <f>N2 &amp; " (" &amp; N7 &amp; ", " &amp; N12 &amp; ")"</f>
+        <f t="shared" si="1"/>
         <v>E (GP3, GP22)</v>
       </c>
       <c r="O17" s="21" t="str">
-        <f>O2 &amp; " (" &amp; O7 &amp; ", " &amp; O12 &amp; ")"</f>
+        <f t="shared" si="1"/>
         <v>R (GP4, GP22)</v>
       </c>
       <c r="P17" s="21" t="str">
-        <f>P2 &amp; " (" &amp; P7 &amp; ", " &amp; P12 &amp; ")"</f>
+        <f t="shared" si="1"/>
         <v>T (GP5, GP22)</v>
       </c>
       <c r="Q17" s="21" t="str">
-        <f>Q2 &amp; " (" &amp; Q7 &amp; ", " &amp; Q12 &amp; ")"</f>
+        <f t="shared" si="1"/>
         <v>Y (GP5, GP15)</v>
       </c>
       <c r="R17" s="21" t="str">
-        <f>R2 &amp; " (" &amp; R7 &amp; ", " &amp; R12 &amp; ")"</f>
+        <f t="shared" si="1"/>
         <v>U (GP4, GP15)</v>
       </c>
       <c r="S17" s="21" t="str">
-        <f>S2 &amp; " (" &amp; S7 &amp; ", " &amp; S12 &amp; ")"</f>
+        <f t="shared" si="1"/>
         <v>I (GP3, GP15)</v>
       </c>
       <c r="T17" s="21" t="str">
-        <f>T2 &amp; " (" &amp; T7 &amp; ", " &amp; T12 &amp; ")"</f>
+        <f t="shared" si="1"/>
         <v>O (GP2, GP15)</v>
       </c>
       <c r="U17" s="21" t="str">
-        <f>U2 &amp; " (" &amp; U7 &amp; ", " &amp; U12 &amp; ")"</f>
+        <f t="shared" si="1"/>
         <v>P (GP1, GP15)</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="str">
-        <f>A3 &amp; " (" &amp; A8 &amp; ", " &amp; A13 &amp; ")"</f>
+        <f t="shared" ref="A18:J18" si="2">A3 &amp; " (" &amp; A8 &amp; ", " &amp; A13 &amp; ")"</f>
         <v>A (0, 4)</v>
       </c>
       <c r="B18" s="21" t="str">
-        <f>B3 &amp; " (" &amp; B8 &amp; ", " &amp; B13 &amp; ")"</f>
+        <f t="shared" si="2"/>
         <v>S (1, 4)</v>
       </c>
       <c r="C18" s="21" t="str">
-        <f>C3 &amp; " (" &amp; C8 &amp; ", " &amp; C13 &amp; ")"</f>
+        <f t="shared" si="2"/>
         <v>D (2, 4)</v>
       </c>
       <c r="D18" s="21" t="str">
-        <f>D3 &amp; " (" &amp; D8 &amp; ", " &amp; D13 &amp; ")"</f>
+        <f t="shared" si="2"/>
         <v>F (3, 4)</v>
       </c>
       <c r="E18" s="21" t="str">
-        <f>E3 &amp; " (" &amp; E8 &amp; ", " &amp; E13 &amp; ")"</f>
+        <f t="shared" si="2"/>
         <v>G (4, 4)</v>
       </c>
       <c r="F18" s="21" t="str">
-        <f>F3 &amp; " (" &amp; F8 &amp; ", " &amp; F13 &amp; ")"</f>
+        <f t="shared" si="2"/>
         <v>H (4, 1)</v>
       </c>
       <c r="G18" s="21" t="str">
-        <f>G3 &amp; " (" &amp; G8 &amp; ", " &amp; G13 &amp; ")"</f>
+        <f t="shared" si="2"/>
         <v>J (3, 1)</v>
       </c>
       <c r="H18" s="21" t="str">
-        <f>H3 &amp; " (" &amp; H8 &amp; ", " &amp; H13 &amp; ")"</f>
+        <f t="shared" si="2"/>
         <v>K (2, 1)</v>
       </c>
       <c r="I18" s="21" t="str">
-        <f>I3 &amp; " (" &amp; I8 &amp; ", " &amp; I13 &amp; ")"</f>
+        <f t="shared" si="2"/>
         <v>L (1, 1)</v>
       </c>
       <c r="J18" s="21" t="str">
-        <f>J3 &amp; " (" &amp; J8 &amp; ", " &amp; J13 &amp; ")"</f>
+        <f t="shared" si="2"/>
         <v>DEL (0, 1)</v>
       </c>
       <c r="L18" s="21" t="str">
-        <f>L3 &amp; " (" &amp; L8 &amp; ", " &amp; L13 &amp; ")"</f>
+        <f t="shared" ref="L18:U18" si="3">L3 &amp; " (" &amp; L8 &amp; ", " &amp; L13 &amp; ")"</f>
         <v>A (GP1, GP7)</v>
       </c>
       <c r="M18" s="21" t="str">
-        <f>M3 &amp; " (" &amp; M8 &amp; ", " &amp; M13 &amp; ")"</f>
+        <f t="shared" si="3"/>
         <v>S (GP2, GP7)</v>
       </c>
       <c r="N18" s="21" t="str">
-        <f>N3 &amp; " (" &amp; N8 &amp; ", " &amp; N13 &amp; ")"</f>
+        <f t="shared" si="3"/>
         <v>D (GP3, GP7)</v>
       </c>
       <c r="O18" s="21" t="str">
-        <f>O3 &amp; " (" &amp; O8 &amp; ", " &amp; O13 &amp; ")"</f>
+        <f t="shared" si="3"/>
         <v>F (GP4, GP7)</v>
       </c>
       <c r="P18" s="21" t="str">
-        <f>P3 &amp; " (" &amp; P8 &amp; ", " &amp; P13 &amp; ")"</f>
+        <f t="shared" si="3"/>
         <v>G (GP5, GP7)</v>
       </c>
       <c r="Q18" s="21" t="str">
-        <f>Q3 &amp; " (" &amp; Q8 &amp; ", " &amp; Q13 &amp; ")"</f>
+        <f t="shared" si="3"/>
         <v>H (GP5, GP9)</v>
       </c>
       <c r="R18" s="21" t="str">
-        <f>R3 &amp; " (" &amp; R8 &amp; ", " &amp; R13 &amp; ")"</f>
+        <f t="shared" si="3"/>
         <v>J (GP4, GP9)</v>
       </c>
       <c r="S18" s="21" t="str">
-        <f>S3 &amp; " (" &amp; S8 &amp; ", " &amp; S13 &amp; ")"</f>
+        <f t="shared" si="3"/>
         <v>K (GP3, GP9)</v>
       </c>
       <c r="T18" s="21" t="str">
-        <f>T3 &amp; " (" &amp; T8 &amp; ", " &amp; T13 &amp; ")"</f>
+        <f t="shared" si="3"/>
         <v>L (GP2, GP9)</v>
       </c>
       <c r="U18" s="21" t="str">
-        <f>U3 &amp; " (" &amp; U8 &amp; ", " &amp; U13 &amp; ")"</f>
+        <f t="shared" si="3"/>
         <v>DEL (GP1, GP9)</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="str">
-        <f>A4 &amp; " (" &amp; A9 &amp; ", " &amp; A14 &amp; ")"</f>
+        <f t="shared" ref="A19:J19" si="4">A4 &amp; " (" &amp; A9 &amp; ", " &amp; A14 &amp; ")"</f>
         <v>ALT (0, 3)</v>
       </c>
       <c r="B19" s="21" t="str">
-        <f>B4 &amp; " (" &amp; B9 &amp; ", " &amp; B14 &amp; ")"</f>
+        <f t="shared" si="4"/>
         <v>Z (1, 3)</v>
       </c>
       <c r="C19" s="21" t="str">
-        <f>C4 &amp; " (" &amp; C9 &amp; ", " &amp; C14 &amp; ")"</f>
+        <f t="shared" si="4"/>
         <v>X (2, 3)</v>
       </c>
       <c r="D19" s="21" t="str">
-        <f>D4 &amp; " (" &amp; D9 &amp; ", " &amp; D14 &amp; ")"</f>
+        <f t="shared" si="4"/>
         <v>C (3, 3)</v>
       </c>
       <c r="E19" s="21" t="str">
-        <f>E4 &amp; " (" &amp; E9 &amp; ", " &amp; E14 &amp; ")"</f>
+        <f t="shared" si="4"/>
         <v>V (4, 3)</v>
       </c>
       <c r="F19" s="21" t="str">
-        <f>F4 &amp; " (" &amp; F9 &amp; ", " &amp; F14 &amp; ")"</f>
+        <f t="shared" si="4"/>
         <v>B (4, 0)</v>
       </c>
       <c r="G19" s="21" t="str">
-        <f>G4 &amp; " (" &amp; G9 &amp; ", " &amp; G14 &amp; ")"</f>
+        <f t="shared" si="4"/>
         <v>N (3, 0)</v>
       </c>
       <c r="H19" s="21" t="str">
-        <f>H4 &amp; " (" &amp; H9 &amp; ", " &amp; H14 &amp; ")"</f>
+        <f t="shared" si="4"/>
         <v>M (2, 0)</v>
       </c>
       <c r="I19" s="21" t="str">
-        <f>I4 &amp; " (" &amp; I9 &amp; ", " &amp; I14 &amp; ")"</f>
+        <f t="shared" si="4"/>
         <v>SPC (1, 0)</v>
       </c>
       <c r="J19" s="21" t="str">
-        <f>J4 &amp; " (" &amp; J9 &amp; ", " &amp; J14 &amp; ")"</f>
+        <f t="shared" si="4"/>
         <v>ENT (0, 0)</v>
       </c>
       <c r="L19" s="21" t="str">
-        <f>L4 &amp; " (" &amp; L9 &amp; ", " &amp; L14 &amp; ")"</f>
+        <f t="shared" ref="L19:U19" si="5">L4 &amp; " (" &amp; L9 &amp; ", " &amp; L14 &amp; ")"</f>
         <v>ALT (GP1, GP8)</v>
       </c>
       <c r="M19" s="21" t="str">
-        <f>M4 &amp; " (" &amp; M9 &amp; ", " &amp; M14 &amp; ")"</f>
+        <f t="shared" si="5"/>
         <v>Z (GP2, GP8)</v>
       </c>
       <c r="N19" s="21" t="str">
-        <f>N4 &amp; " (" &amp; N9 &amp; ", " &amp; N14 &amp; ")"</f>
+        <f t="shared" si="5"/>
         <v>X (GP3, GP8)</v>
       </c>
       <c r="O19" s="21" t="str">
-        <f>O4 &amp; " (" &amp; O9 &amp; ", " &amp; O14 &amp; ")"</f>
+        <f t="shared" si="5"/>
         <v>C (GP4, GP8)</v>
       </c>
       <c r="P19" s="21" t="str">
-        <f>P4 &amp; " (" &amp; P9 &amp; ", " &amp; P14 &amp; ")"</f>
+        <f t="shared" si="5"/>
         <v>V (GP5, GP8)</v>
       </c>
       <c r="Q19" s="21" t="str">
-        <f>Q4 &amp; " (" &amp; Q9 &amp; ", " &amp; Q14 &amp; ")"</f>
+        <f t="shared" si="5"/>
         <v>B (GP5, GP6)</v>
       </c>
       <c r="R19" s="21" t="str">
-        <f>R4 &amp; " (" &amp; R9 &amp; ", " &amp; R14 &amp; ")"</f>
+        <f t="shared" si="5"/>
         <v>N (GP4, GP6)</v>
       </c>
       <c r="S19" s="21" t="str">
-        <f>S4 &amp; " (" &amp; S9 &amp; ", " &amp; S14 &amp; ")"</f>
+        <f t="shared" si="5"/>
         <v>M (GP3, GP6)</v>
       </c>
       <c r="T19" s="21" t="str">
-        <f>T4 &amp; " (" &amp; T9 &amp; ", " &amp; T14 &amp; ")"</f>
+        <f t="shared" si="5"/>
         <v>SPC (GP2, GP6)</v>
       </c>
       <c r="U19" s="21" t="str">
-        <f>U4 &amp; " (" &amp; U9 &amp; ", " &amp; U14 &amp; ")"</f>
+        <f t="shared" si="5"/>
         <v>ENT (GP1, GP6)</v>
       </c>
     </row>
@@ -4135,7 +4193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638AD3B4-41B9-45BA-A561-4767E27251F2}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -4291,4 +4349,185 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5A7B195-9A8E-4431-8B4B-D79010CDB109}">
+  <dimension ref="A1:P5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23">
+        <v>2</v>
+      </c>
+      <c r="D1" s="23">
+        <v>3</v>
+      </c>
+      <c r="E1" s="23">
+        <v>4</v>
+      </c>
+      <c r="F1" s="23">
+        <v>5</v>
+      </c>
+      <c r="G1" s="23">
+        <v>6</v>
+      </c>
+      <c r="H1" s="23">
+        <v>7</v>
+      </c>
+      <c r="I1" s="23">
+        <v>8</v>
+      </c>
+      <c r="J1" s="23">
+        <v>9</v>
+      </c>
+      <c r="K1" s="23">
+        <v>10</v>
+      </c>
+      <c r="L1" s="23">
+        <v>11</v>
+      </c>
+      <c r="M1" s="23">
+        <v>12</v>
+      </c>
+      <c r="N1" s="23">
+        <v>13</v>
+      </c>
+      <c r="O1" s="23">
+        <v>14</v>
+      </c>
+      <c r="P1" s="23">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>13121100</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3020101</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F3" s="1">
+        <v>-9.8000000000000007</v>
+      </c>
+      <c r="G3" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="H3" s="1">
+        <v>21.620999999999999</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D5" t="s">
+        <v>240</v>
+      </c>
+      <c r="E5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F5" t="s">
+        <v>241</v>
+      </c>
+      <c r="G5" t="s">
+        <v>242</v>
+      </c>
+      <c r="H5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>